<commit_message>
created more complex task creation with a number of form elements, commiting before substantial change to form class/
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint1 18.11.19.xlsx
+++ b/Planning Report/application sprint planner sprint1 18.11.19.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C4064F-354B-453F-81D5-C8A83554ECC7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9C5CED-06D3-4BB3-A514-8E139108EAE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="28200" windowHeight="14085" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -1355,6 +1355,40 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="92">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2860,40 +2894,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3215,10 +3215,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
@@ -3498,8 +3498,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8729,7 +8729,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="32"/>
       <c r="H28" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28" s="26"/>
       <c r="J28" s="38" t="str">
@@ -10837,7 +10837,9 @@
         <v>4</v>
       </c>
       <c r="F40" s="31"/>
-      <c r="G40" s="32"/>
+      <c r="G40" s="32">
+        <v>43789</v>
+      </c>
       <c r="H40" s="33">
         <v>1</v>
       </c>
@@ -11082,7 +11084,9 @@
         <v>2</v>
       </c>
       <c r="F41" s="31"/>
-      <c r="G41" s="32"/>
+      <c r="G41" s="32">
+        <v>43789</v>
+      </c>
       <c r="H41" s="33">
         <v>1</v>
       </c>
@@ -22904,56 +22908,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:BM8 J96:BM97 J68:BM71 J77:BM77 J53:BM53 J74:BM74 J83:BM83 J63:BM66 J55:BM56 J10:BM10 J45:BM50 J22:BM43">
-    <cfRule type="expression" dxfId="75" priority="243">
+    <cfRule type="expression" dxfId="79" priority="243">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="74" priority="249">
+    <cfRule type="expression" dxfId="78" priority="249">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:BM4">
-    <cfRule type="expression" dxfId="73" priority="245">
+    <cfRule type="expression" dxfId="77" priority="245">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BM4">
-    <cfRule type="expression" dxfId="72" priority="244">
+    <cfRule type="expression" dxfId="76" priority="244">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:BM8 J10:BM10 J22:BM96">
-    <cfRule type="expression" dxfId="71" priority="266" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="266" stopIfTrue="1">
       <formula>AND($D8="Low risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="285" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="285" stopIfTrue="1">
       <formula>AND($D8="High risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="303" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="303" stopIfTrue="1">
       <formula>AND($D8="On track",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="304" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="304" stopIfTrue="1">
       <formula>AND($D8="Med risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="305" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="305" stopIfTrue="1">
       <formula>AND(LEN($D8)=0,J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J97:BM97">
-    <cfRule type="expression" dxfId="66" priority="313" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="313" stopIfTrue="1">
       <formula>AND(#REF!="Low risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="314" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="314" stopIfTrue="1">
       <formula>AND(#REF!="High risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="315" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="315" stopIfTrue="1">
       <formula>AND(#REF!="On track",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="316" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="316" stopIfTrue="1">
       <formula>AND(#REF!="Med risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="317" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="317" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22972,24 +22976,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="61" priority="234">
+    <cfRule type="expression" dxfId="65" priority="234">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="60" priority="236" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="236" stopIfTrue="1">
       <formula>AND($D9="Low risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="237" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="237" stopIfTrue="1">
       <formula>AND($D9="High risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="238" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="238" stopIfTrue="1">
       <formula>AND($D9="On track",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="239" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="239" stopIfTrue="1">
       <formula>AND($D9="Med risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="240" stopIfTrue="1">
       <formula>AND(LEN($D9)=0,J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23008,7 +23012,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J60:BM60 J57:BM58">
-    <cfRule type="expression" dxfId="55" priority="218">
+    <cfRule type="expression" dxfId="59" priority="218">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23027,7 +23031,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J62:GC62">
-    <cfRule type="expression" dxfId="54" priority="209">
+    <cfRule type="expression" dxfId="58" priority="209">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23046,7 +23050,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J61:BM61 J59:BM59">
-    <cfRule type="expression" dxfId="53" priority="202">
+    <cfRule type="expression" dxfId="57" priority="202">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23065,7 +23069,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:BM44">
-    <cfRule type="expression" dxfId="52" priority="194">
+    <cfRule type="expression" dxfId="56" priority="194">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23084,7 +23088,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J67:GC67">
-    <cfRule type="expression" dxfId="51" priority="185">
+    <cfRule type="expression" dxfId="55" priority="185">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23103,7 +23107,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J78:GC79 J81:GC83 J86:GC86 J93:GC95">
-    <cfRule type="expression" dxfId="50" priority="178">
+    <cfRule type="expression" dxfId="54" priority="178">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23122,7 +23126,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J80:GC80">
-    <cfRule type="expression" dxfId="49" priority="170">
+    <cfRule type="expression" dxfId="53" priority="170">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23141,7 +23145,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:GC76">
-    <cfRule type="expression" dxfId="48" priority="161">
+    <cfRule type="expression" dxfId="52" priority="161">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23160,7 +23164,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:GC52">
-    <cfRule type="expression" dxfId="47" priority="153">
+    <cfRule type="expression" dxfId="51" priority="153">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23179,7 +23183,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73:BM73">
-    <cfRule type="expression" dxfId="46" priority="145">
+    <cfRule type="expression" dxfId="50" priority="145">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23198,7 +23202,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J84:GC85">
-    <cfRule type="expression" dxfId="45" priority="137">
+    <cfRule type="expression" dxfId="49" priority="137">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23217,7 +23221,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87:GC88">
-    <cfRule type="expression" dxfId="44" priority="129">
+    <cfRule type="expression" dxfId="48" priority="129">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23236,7 +23240,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J91:GC91">
-    <cfRule type="expression" dxfId="43" priority="121">
+    <cfRule type="expression" dxfId="47" priority="121">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23255,7 +23259,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92:GC92">
-    <cfRule type="expression" dxfId="42" priority="113">
+    <cfRule type="expression" dxfId="46" priority="113">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23274,7 +23278,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:BM75">
-    <cfRule type="expression" dxfId="41" priority="105">
+    <cfRule type="expression" dxfId="45" priority="105">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23293,7 +23297,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:BM54">
-    <cfRule type="expression" dxfId="40" priority="97">
+    <cfRule type="expression" dxfId="44" priority="97">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23312,7 +23316,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J90:BM90">
-    <cfRule type="expression" dxfId="39" priority="89">
+    <cfRule type="expression" dxfId="43" priority="89">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23331,7 +23335,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J72:BM72">
-    <cfRule type="expression" dxfId="38" priority="57">
+    <cfRule type="expression" dxfId="42" priority="57">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23350,12 +23354,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89:GC89">
-    <cfRule type="expression" dxfId="37" priority="65">
+    <cfRule type="expression" dxfId="41" priority="65">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:BM51">
-    <cfRule type="expression" dxfId="36" priority="49">
+    <cfRule type="expression" dxfId="40" priority="49">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23388,24 +23392,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="35" priority="41">
+    <cfRule type="expression" dxfId="39" priority="41">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="34" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="43" stopIfTrue="1">
       <formula>AND($D11="Low risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="44" stopIfTrue="1">
       <formula>AND($D11="High risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="45" stopIfTrue="1">
       <formula>AND($D11="On track",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="46" stopIfTrue="1">
       <formula>AND($D11="Med risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="47" stopIfTrue="1">
       <formula>AND(LEN($D11)=0,J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23424,24 +23428,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="29" priority="33">
+    <cfRule type="expression" dxfId="33" priority="33">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="28" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
       <formula>AND($D12="Low risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="36" stopIfTrue="1">
       <formula>AND($D12="High risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="37" stopIfTrue="1">
       <formula>AND($D12="On track",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="38" stopIfTrue="1">
       <formula>AND($D12="Med risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="39" stopIfTrue="1">
       <formula>AND(LEN($D12)=0,J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23460,24 +23464,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>AND($D15="Low risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="28" stopIfTrue="1">
       <formula>AND($D15="High risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="29" stopIfTrue="1">
       <formula>AND($D15="On track",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="30" stopIfTrue="1">
       <formula>AND($D15="Med risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="31" stopIfTrue="1">
       <formula>AND(LEN($D15)=0,J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23496,46 +23500,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="21" priority="17">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
       <formula>AND($D16="Low risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
       <formula>AND($D16="High risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
       <formula>AND($D16="On track",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="22" stopIfTrue="1">
       <formula>AND($D16="Med risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="23" stopIfTrue="1">
       <formula>AND(LEN($D16)=0,J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="12" stopIfTrue="1">
       <formula>AND($D19="Low risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
       <formula>AND($D19="High risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
       <formula>AND($D19="On track",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>AND($D19="Med risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
       <formula>AND(LEN($D19)=0,J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23554,19 +23558,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:BM21">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>AND($D20="Low risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="5" stopIfTrue="1">
       <formula>AND($D20="High risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="6" stopIfTrue="1">
       <formula>AND($D20="On track",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>AND($D20="Med risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
       <formula>AND(LEN($D20)=0,J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23585,7 +23589,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:GC21">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
created class diagrams for the first release.
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint1 18.11.19.xlsx
+++ b/Planning Report/application sprint planner sprint1 18.11.19.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9C5CED-06D3-4BB3-A514-8E139108EAE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDF7A2A-F589-467E-9659-9557DBF1155D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="28200" windowHeight="14085" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="99">
   <si>
     <t>Create a Gantt Chart in this worksheet.
 Enter title of this project in cell B1. 
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Task Creation</t>
+  </si>
+  <si>
+    <t>VIVA</t>
   </si>
 </sst>
 </file>
@@ -1355,40 +1358,6 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="92">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2894,6 +2863,40 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3215,10 +3218,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="76"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
@@ -3498,8 +3501,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8726,10 +8729,14 @@
       <c r="E28" s="34">
         <v>2</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="32"/>
+      <c r="F28" s="31">
+        <v>1</v>
+      </c>
+      <c r="G28" s="32">
+        <v>43795</v>
+      </c>
       <c r="H28" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I28" s="26"/>
       <c r="J28" s="38" t="str">
@@ -10358,7 +10365,9 @@
       <c r="E36" s="34">
         <v>0.5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="31">
+        <v>1</v>
+      </c>
       <c r="G36" s="32">
         <v>43788</v>
       </c>
@@ -10426,7 +10435,7 @@
     <row r="37" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="41" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="C37" s="41" t="s">
         <v>67</v>
@@ -10437,8 +10446,12 @@
       <c r="E37" s="34">
         <v>0.5</v>
       </c>
-      <c r="F37" s="31"/>
-      <c r="G37" s="32"/>
+      <c r="F37" s="31">
+        <v>1</v>
+      </c>
+      <c r="G37" s="32">
+        <v>43797</v>
+      </c>
       <c r="H37" s="33">
         <v>1</v>
       </c>
@@ -10509,13 +10522,17 @@
         <v>67</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E38" s="34">
         <v>4</v>
       </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="32"/>
+      <c r="F38" s="31">
+        <v>1</v>
+      </c>
+      <c r="G38" s="32">
+        <v>43795</v>
+      </c>
       <c r="H38" s="33">
         <v>1</v>
       </c>
@@ -10836,7 +10853,9 @@
       <c r="E40" s="34">
         <v>4</v>
       </c>
-      <c r="F40" s="31"/>
+      <c r="F40" s="31">
+        <v>1</v>
+      </c>
       <c r="G40" s="32">
         <v>43789</v>
       </c>
@@ -22908,56 +22927,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:BM8 J96:BM97 J68:BM71 J77:BM77 J53:BM53 J74:BM74 J83:BM83 J63:BM66 J55:BM56 J10:BM10 J45:BM50 J22:BM43">
-    <cfRule type="expression" dxfId="79" priority="243">
+    <cfRule type="expression" dxfId="75" priority="243">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="78" priority="249">
+    <cfRule type="expression" dxfId="74" priority="249">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:BM4">
-    <cfRule type="expression" dxfId="77" priority="245">
+    <cfRule type="expression" dxfId="73" priority="245">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BM4">
-    <cfRule type="expression" dxfId="76" priority="244">
+    <cfRule type="expression" dxfId="72" priority="244">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:BM8 J10:BM10 J22:BM96">
-    <cfRule type="expression" dxfId="75" priority="266" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="266" stopIfTrue="1">
       <formula>AND($D8="Low risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="285" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="285" stopIfTrue="1">
       <formula>AND($D8="High risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="303" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="303" stopIfTrue="1">
       <formula>AND($D8="On track",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="304" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="304" stopIfTrue="1">
       <formula>AND($D8="Med risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="305" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="305" stopIfTrue="1">
       <formula>AND(LEN($D8)=0,J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J97:BM97">
-    <cfRule type="expression" dxfId="70" priority="313" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="313" stopIfTrue="1">
       <formula>AND(#REF!="Low risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="314" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="314" stopIfTrue="1">
       <formula>AND(#REF!="High risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="315" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="315" stopIfTrue="1">
       <formula>AND(#REF!="On track",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="316" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="316" stopIfTrue="1">
       <formula>AND(#REF!="Med risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="317" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="317" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22976,24 +22995,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="65" priority="234">
+    <cfRule type="expression" dxfId="61" priority="234">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="64" priority="236" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="236" stopIfTrue="1">
       <formula>AND($D9="Low risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="237" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="237" stopIfTrue="1">
       <formula>AND($D9="High risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="238" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="238" stopIfTrue="1">
       <formula>AND($D9="On track",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="239" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="239" stopIfTrue="1">
       <formula>AND($D9="Med risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="240" stopIfTrue="1">
       <formula>AND(LEN($D9)=0,J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23012,7 +23031,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J60:BM60 J57:BM58">
-    <cfRule type="expression" dxfId="59" priority="218">
+    <cfRule type="expression" dxfId="55" priority="218">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23031,7 +23050,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J62:GC62">
-    <cfRule type="expression" dxfId="58" priority="209">
+    <cfRule type="expression" dxfId="54" priority="209">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23050,7 +23069,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J61:BM61 J59:BM59">
-    <cfRule type="expression" dxfId="57" priority="202">
+    <cfRule type="expression" dxfId="53" priority="202">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23069,7 +23088,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:BM44">
-    <cfRule type="expression" dxfId="56" priority="194">
+    <cfRule type="expression" dxfId="52" priority="194">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23088,7 +23107,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J67:GC67">
-    <cfRule type="expression" dxfId="55" priority="185">
+    <cfRule type="expression" dxfId="51" priority="185">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23107,7 +23126,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J78:GC79 J81:GC83 J86:GC86 J93:GC95">
-    <cfRule type="expression" dxfId="54" priority="178">
+    <cfRule type="expression" dxfId="50" priority="178">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23126,7 +23145,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J80:GC80">
-    <cfRule type="expression" dxfId="53" priority="170">
+    <cfRule type="expression" dxfId="49" priority="170">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23145,7 +23164,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:GC76">
-    <cfRule type="expression" dxfId="52" priority="161">
+    <cfRule type="expression" dxfId="48" priority="161">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23164,7 +23183,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:GC52">
-    <cfRule type="expression" dxfId="51" priority="153">
+    <cfRule type="expression" dxfId="47" priority="153">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23183,7 +23202,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73:BM73">
-    <cfRule type="expression" dxfId="50" priority="145">
+    <cfRule type="expression" dxfId="46" priority="145">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23202,7 +23221,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J84:GC85">
-    <cfRule type="expression" dxfId="49" priority="137">
+    <cfRule type="expression" dxfId="45" priority="137">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23221,7 +23240,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87:GC88">
-    <cfRule type="expression" dxfId="48" priority="129">
+    <cfRule type="expression" dxfId="44" priority="129">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23240,7 +23259,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J91:GC91">
-    <cfRule type="expression" dxfId="47" priority="121">
+    <cfRule type="expression" dxfId="43" priority="121">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23259,7 +23278,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92:GC92">
-    <cfRule type="expression" dxfId="46" priority="113">
+    <cfRule type="expression" dxfId="42" priority="113">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23278,7 +23297,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:BM75">
-    <cfRule type="expression" dxfId="45" priority="105">
+    <cfRule type="expression" dxfId="41" priority="105">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23297,7 +23316,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:BM54">
-    <cfRule type="expression" dxfId="44" priority="97">
+    <cfRule type="expression" dxfId="40" priority="97">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23316,7 +23335,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J90:BM90">
-    <cfRule type="expression" dxfId="43" priority="89">
+    <cfRule type="expression" dxfId="39" priority="89">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23335,7 +23354,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J72:BM72">
-    <cfRule type="expression" dxfId="42" priority="57">
+    <cfRule type="expression" dxfId="38" priority="57">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23354,12 +23373,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89:GC89">
-    <cfRule type="expression" dxfId="41" priority="65">
+    <cfRule type="expression" dxfId="37" priority="65">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:BM51">
-    <cfRule type="expression" dxfId="40" priority="49">
+    <cfRule type="expression" dxfId="36" priority="49">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23392,24 +23411,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="39" priority="41">
+    <cfRule type="expression" dxfId="35" priority="41">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="38" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="43" stopIfTrue="1">
       <formula>AND($D11="Low risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="44" stopIfTrue="1">
       <formula>AND($D11="High risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="45" stopIfTrue="1">
       <formula>AND($D11="On track",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="46" stopIfTrue="1">
       <formula>AND($D11="Med risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="47" stopIfTrue="1">
       <formula>AND(LEN($D11)=0,J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23428,24 +23447,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="33" priority="33">
+    <cfRule type="expression" dxfId="29" priority="33">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="35" stopIfTrue="1">
       <formula>AND($D12="Low risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="36" stopIfTrue="1">
       <formula>AND($D12="High risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="37" stopIfTrue="1">
       <formula>AND($D12="On track",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="38" stopIfTrue="1">
       <formula>AND($D12="Med risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="39" stopIfTrue="1">
       <formula>AND(LEN($D12)=0,J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23464,24 +23483,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="27" priority="25">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
       <formula>AND($D15="Low risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="28" stopIfTrue="1">
       <formula>AND($D15="High risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="29" stopIfTrue="1">
       <formula>AND($D15="On track",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="30" stopIfTrue="1">
       <formula>AND($D15="Med risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="31" stopIfTrue="1">
       <formula>AND(LEN($D15)=0,J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23500,46 +23519,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="21" priority="17">
+    <cfRule type="expression" dxfId="17" priority="17">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>AND($D16="Low risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="20" stopIfTrue="1">
       <formula>AND($D16="High risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="21" stopIfTrue="1">
       <formula>AND($D16="On track",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="22" stopIfTrue="1">
       <formula>AND($D16="Med risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="23" stopIfTrue="1">
       <formula>AND(LEN($D16)=0,J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="15" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
       <formula>AND($D19="Low risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
       <formula>AND($D19="High risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="14" stopIfTrue="1">
       <formula>AND($D19="On track",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="15" stopIfTrue="1">
       <formula>AND($D19="Med risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="16" stopIfTrue="1">
       <formula>AND(LEN($D19)=0,J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23558,19 +23577,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:BM21">
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>AND($D20="Low risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>AND($D20="High risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
       <formula>AND($D20="On track",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
       <formula>AND($D20="Med risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
       <formula>AND(LEN($D20)=0,J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23589,7 +23608,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:GC21">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>